<commit_message>
implementando modulo para buscar informações  fiscais da encomenda gerada
</commit_message>
<xml_diff>
--- a/bases/planilha Base.xlsx
+++ b/bases/planilha Base.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dato\Documents\REPOSITÓRIO\Gerar e Rastrear encomendas - Buslog\bases\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF66605-5521-4426-A564-6BD0D6169169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-28908" yWindow="-108" windowWidth="29016" windowHeight="15696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Planilha1"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>FRAQUIA</t>
   </si>
@@ -25,23 +44,22 @@
     <t>CTE</t>
   </si>
   <si>
+    <t>dato-teste-valor</t>
+  </si>
+  <si>
     <t>BUSLOG-SUBWAY</t>
   </si>
   <si>
-    <t>Entregue</t>
+    <t>pendente</t>
   </si>
   <si>
-    <t>Em Rota</t>
-  </si>
-  <si>
-    <t>TRANSFERENCIA</t>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -53,14 +71,14 @@
     <font>
       <b/>
       <sz val="8"/>
-      <color rgb="FFffffff"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
-      <color rgb="FFffffff"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -92,7 +110,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -113,12 +131,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0e2841"/>
+        <fgColor rgb="FF0E2841"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF80350e"/>
+        <fgColor rgb="FF80350E"/>
       </patternFill>
     </fill>
     <fill>
@@ -128,12 +146,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF61cbf4"/>
+        <fgColor rgb="FF61CBF4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -156,7 +174,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -165,13 +183,13 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -192,7 +210,7 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -201,7 +219,7 @@
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -220,7 +238,7 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -245,70 +263,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="6" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="6" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -319,10 +340,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -360,71 +381,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -452,7 +473,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -475,11 +496,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -488,13 +509,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -504,7 +525,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -513,7 +534,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -522,7 +543,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -530,10 +551,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -598,23 +619,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="17" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="18" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,103 +651,88 @@
         <v>45469</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="5">
-        <v>58398</v>
+    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="7">
+        <v>758048</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7">
-        <v>360133</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="5">
-        <v>58399</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="C3" s="7">
-        <v>360147</v>
+        <v>761822</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="5">
-        <v>58414</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7">
-        <v>360081</v>
-      </c>
-      <c r="D4" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="5">
-        <v>58415</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7">
-        <v>362031</v>
-      </c>
-      <c r="D5" s="8" t="s">
+    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="9"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="11"/>
+      <c r="D4" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="13"/>
+    </row>
+    <row r="8" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>